<commit_message>
Added another column that combines all the addresses in the correct format accepted by the program
</commit_message>
<xml_diff>
--- a/Sample Data for TSP Project.xlsx
+++ b/Sample Data for TSP Project.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\James Laptop\Lecture Notes\Second Year\2nd Semester\CS211\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Backup laptop vechi\Lecture Notes\Second Year\2nd Semester\CS211\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADAA8EC-A6DF-4BA8-80DB-4E0E1C2A80F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13290" windowHeight="8970"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>ADDRESS</t>
   </si>
@@ -38,9 +47,6 @@
     <t>GPS West</t>
   </si>
   <si>
-    <t xml:space="preserve">38 Parsons Hall Maynooth </t>
-  </si>
-  <si>
     <t xml:space="preserve">34 Silken Vale Maynooth </t>
   </si>
   <si>
@@ -156,12 +162,138 @@
   </si>
   <si>
     <t xml:space="preserve">18 College Green Maynooth </t>
+  </si>
+  <si>
+    <t>1,38 Parsons Hall Maynooth 4,53.37521,-6.6103</t>
+  </si>
+  <si>
+    <t>2,34 Silken Vale Maynooth 6,53.37626,-6.59308</t>
+  </si>
+  <si>
+    <t>3,156 Glendale Leixlip 18,53.37077,-6.48279</t>
+  </si>
+  <si>
+    <t>4,33 The Paddocks Oldtown Mill Celbridge 8,53.3473,-6.55057</t>
+  </si>
+  <si>
+    <t>5,902 Lady Castle K Club Straffan 11,53.31159,-6.60538</t>
+  </si>
+  <si>
+    <t>6,9 The Park Louisa Valley Leixlip 3,53.36115,-6.48907</t>
+  </si>
+  <si>
+    <t>7,509 Riverforest Leixlip 10,53.37402,-6.49363</t>
+  </si>
+  <si>
+    <t>8,16 Priory Chase St.Raphaels Manor Celbridge 7,53.33886,-6.55468</t>
+  </si>
+  <si>
+    <t>9,13 Abbey Park Court Clane 13,53.2908,-6.67746</t>
+  </si>
+  <si>
+    <t>10,117 Royal Meadows Kilcock 12,53.39459,-6.66995</t>
+  </si>
+  <si>
+    <t>11,7 Riverlawn Abbeyfarm Celbridge 3,53.33239,-6.55163</t>
+  </si>
+  <si>
+    <t>12,10 Fair Green Court Kilccock 7,53.39847,-6.66787</t>
+  </si>
+  <si>
+    <t>13,11 The Lodge Abbeylands Clane 12,53.29128,-6.67836</t>
+  </si>
+  <si>
+    <t>14,628 Riverforest Leixlip 5,53.37416,-6.49731</t>
+  </si>
+  <si>
+    <t>15,12 Castlevillage Avenue Celbridge 8,53.35298,-6.54921</t>
+  </si>
+  <si>
+    <t>16,116 Connaught Street Kilcock 4,53.39839,-6.66767</t>
+  </si>
+  <si>
+    <t>17,44 Rinawade Avenue Leixlip</t>
+  </si>
+  <si>
+    <t>20,53.36141,-6.51834</t>
+  </si>
+  <si>
+    <t>18,35 Beech Park Wood Beech Park Leixlip 14,53.36287,-6.52468</t>
+  </si>
+  <si>
+    <t>19,96 Priory Lodge St. Raphael's Manor Celbridge 2,53.33835,-6.53984</t>
+  </si>
+  <si>
+    <t>20,33 Leinster Wood Carton Demesne Maynooth 7,53.39351,-6.5542</t>
+  </si>
+  <si>
+    <t>21,6 Glen Easton View Leixlip 15,53.36883,-6.51468</t>
+  </si>
+  <si>
+    <t>22,40 Oaklawn West. Leixlip 8,53.36833,-6.50589</t>
+  </si>
+  <si>
+    <t>23,169 Glendale Leixlip 24,53.37043,-6.48193</t>
+  </si>
+  <si>
+    <t>24,14 The Rise Louisa Valley Leixlip 15,53.36115,-6.48907</t>
+  </si>
+  <si>
+    <t>25,28 The Lawn Moyglare Abbey Maynooth 7,53.38895,-6.60579</t>
+  </si>
+  <si>
+    <t>26,43 The Woodlands Castletown Celbridge 12,53.34678,-6.53415</t>
+  </si>
+  <si>
+    <t>27,14 Rye River Crescent Dun Carraig Leixlip 8,53.36518,-6.48913</t>
+  </si>
+  <si>
+    <t>28,32 The View St.Wolstan Abbey Celbridge 10,53.33751,-6.53173</t>
+  </si>
+  <si>
+    <t>29,20 Habourview The Glenroyal Centre Maynooth 9,53.37954,-6.58793</t>
+  </si>
+  <si>
+    <t>30,416A Ballyoulster Celbridge 5,53.34133,-6.51856</t>
+  </si>
+  <si>
+    <t>31,10 Brookfield Avenue Maynooth 8,53.36976,-6.59828</t>
+  </si>
+  <si>
+    <t>32,15 Willow Rise Primrose Gate Celbridge 19,53.33591,-6.53566</t>
+  </si>
+  <si>
+    <t>33,3 Lyreen Park Maynooth 26,53.38579,-6.58673</t>
+  </si>
+  <si>
+    <t>34,2 Beaufield Drive Maynooth 10,53.37414,-6.60028</t>
+  </si>
+  <si>
+    <t>35,28 The Avenue Castletown Celbridge 18,53.34514,-6.53615</t>
+  </si>
+  <si>
+    <t>36,4 Abbey Park Grove Clane 14,53.29206,-6.67685</t>
+  </si>
+  <si>
+    <t>37,78 Crodaun Forest Park Celbridge 15,53.35401,-6.54603</t>
+  </si>
+  <si>
+    <t>38,1 Kyldar House Manor Mills Maynooth 29,53.38122,-6.59226</t>
+  </si>
+  <si>
+    <t>39,1002 Avondale Leixlip 22,53.36869,-6.48314</t>
+  </si>
+  <si>
+    <t>40,18 College Green Maynooth 5,53.37247,-6.60044</t>
+  </si>
+  <si>
+    <t>38 Parsons Hall Maynooth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,11 +652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G2" sqref="G2:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,9 +665,10 @@
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="68.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,12 +682,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2">
         <v>4</v>
@@ -565,14 +698,18 @@
       <c r="E2">
         <v>-6.6102999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2</f>
+        <v>1,38 Parsons Hall Maynooth,4,53.37521,-6.6103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>6</v>
@@ -583,14 +720,18 @@
       <c r="E3">
         <v>-6.5930799999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G41" si="0">A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3</f>
+        <v>2,34 Silken Vale Maynooth ,6,53.37626,-6.59308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A40" si="0">A3+1</f>
+        <f t="shared" ref="A4:A40" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>18</v>
@@ -601,14 +742,18 @@
       <c r="E4">
         <v>-6.4827899999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>3,156 Glendale Leixlip ,18,53.37077,-6.48279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>8</v>
@@ -619,14 +764,18 @@
       <c r="E5">
         <v>-6.5505699999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>4,33 The Paddocks Oldtown Mill Celbridge ,8,53.3473,-6.55057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>11</v>
@@ -637,14 +786,18 @@
       <c r="E6">
         <v>-6.6053800000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>5,902 Lady Castle K Club Straffan ,11,53.31159,-6.60538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>3</v>
@@ -655,14 +808,18 @@
       <c r="E7">
         <v>-6.4890699999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>6,9 The Park Louisa Valley Leixlip ,3,53.36115,-6.48907</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>10</v>
@@ -673,14 +830,18 @@
       <c r="E8">
         <v>-6.4936299999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>7,509 Riverforest Leixlip ,10,53.37402,-6.49363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2">
         <v>7</v>
@@ -691,14 +852,18 @@
       <c r="E9">
         <v>-6.5546800000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>8,16 Priory Chase St.Raphaels Manor Celbridge ,7,53.33886,-6.55468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2">
         <v>13</v>
@@ -709,14 +874,18 @@
       <c r="E10">
         <v>-6.67746</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>9,13 Abbey Park Court Clane,13,53.2908,-6.67746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <v>12</v>
@@ -727,14 +896,18 @@
       <c r="E11">
         <v>-6.66995</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>10,117 Royal Meadows Kilcock ,12,53.39459,-6.66995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
@@ -745,14 +918,18 @@
       <c r="E12">
         <v>-6.5516300000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>11,7 Riverlawn Abbeyfarm Celbridge ,3,53.33239,-6.55163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
         <v>7</v>
@@ -763,14 +940,18 @@
       <c r="E13">
         <v>-6.6678699999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>12,10 Fair Green Court Kilccock ,7,53.39847,-6.66787</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>12</v>
@@ -781,14 +962,18 @@
       <c r="E14">
         <v>-6.6783599999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>13,11 The Lodge Abbeylands Clane,12,53.29128,-6.67836</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
@@ -799,14 +984,18 @@
       <c r="E15">
         <v>-6.4973099999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>14,628 Riverforest Leixlip ,5,53.37416,-6.49731</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2">
         <v>8</v>
@@ -817,14 +1006,18 @@
       <c r="E16">
         <v>-6.5492100000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>15,12 Castlevillage Avenue Celbridge ,8,53.35298,-6.54921</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2">
         <v>4</v>
@@ -835,14 +1028,18 @@
       <c r="E17">
         <v>-6.6676700000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>16,116 Connaught Street Kilcock ,4,53.39839,-6.66767</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
         <v>20</v>
@@ -853,14 +1050,18 @@
       <c r="E18">
         <v>-6.5183400000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>17,44 Rinawade Avenue Leixlip ,20,53.36141,-6.51834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2">
         <v>14</v>
@@ -871,14 +1072,18 @@
       <c r="E19">
         <v>-6.52468</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>18,35 Beech Park Wood Beech Park Leixlip ,14,53.36287,-6.52468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -889,14 +1094,18 @@
       <c r="E20">
         <v>-6.5398399999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>19,96 Priory Lodge St. Raphael's Manor Celbridge ,2,53.33835,-6.53984</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2">
         <v>7</v>
@@ -907,14 +1116,18 @@
       <c r="E21">
         <v>-6.5541999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>20,33 Leinster Wood Carton Demesne Maynooth ,7,53.39351,-6.5542</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2">
         <v>15</v>
@@ -925,14 +1138,18 @@
       <c r="E22">
         <v>-6.5146800000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f>A22&amp;","&amp;B22&amp;","&amp;C22&amp;","&amp;D22&amp;","&amp;E22</f>
+        <v>21,6 Glen Easton View Leixlip ,15,53.36883,-6.51468</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2">
         <v>8</v>
@@ -943,14 +1160,18 @@
       <c r="E23">
         <v>-6.50589</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>22,40 Oaklawn West. Leixlip ,8,53.36833,-6.50589</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2">
         <v>24</v>
@@ -961,14 +1182,18 @@
       <c r="E24">
         <v>-6.4819300000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>23,169 Glendale Leixlip ,24,53.37043,-6.48193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2">
         <v>15</v>
@@ -979,14 +1204,18 @@
       <c r="E25">
         <v>-6.4890699999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>24,14 The Rise Louisa Valley Leixlip ,15,53.36115,-6.48907</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2">
         <v>7</v>
@@ -997,14 +1226,18 @@
       <c r="E26">
         <v>-6.6057899999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>25,28 The Lawn Moyglare Abbey Maynooth ,7,53.38895,-6.60579</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2">
         <v>12</v>
@@ -1015,14 +1248,18 @@
       <c r="E27">
         <v>-6.5341500000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>26,43 The Woodlands Castletown Celbridge ,12,53.34678,-6.53415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2">
         <v>8</v>
@@ -1033,14 +1270,18 @@
       <c r="E28">
         <v>-6.4891300000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>27,14 Rye River Crescent Dun Carraig Leixlip ,8,53.36518,-6.48913</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2">
         <v>10</v>
@@ -1051,14 +1292,18 @@
       <c r="E29">
         <v>-6.5317299999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>28,32 The View St.Wolstan Abbey Celbridge ,10,53.33751,-6.53173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2">
         <v>9</v>
@@ -1069,14 +1314,18 @@
       <c r="E30">
         <v>-6.5879300000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>29,20 Habourview The Glenroyal Centre Maynooth ,9,53.37954,-6.58793</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2">
         <v>5</v>
@@ -1087,14 +1336,18 @@
       <c r="E31">
         <v>-6.5185599999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>30,416A Ballyoulster Celbridge ,5,53.34133,-6.51856</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2">
         <v>8</v>
@@ -1105,14 +1358,18 @@
       <c r="E32">
         <v>-6.5982799999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>31,10 Brookfield Avenue Maynooth ,8,53.36976,-6.59828</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2">
         <v>19</v>
@@ -1123,14 +1380,18 @@
       <c r="E33">
         <v>-6.53566</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>32,15 Willow Rise Primrose Gate Celbridge ,19,53.33591,-6.53566</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="2">
         <v>26</v>
@@ -1141,14 +1402,18 @@
       <c r="E34">
         <v>-6.5867300000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>33,3 Lyreen Park Maynooth ,26,53.38579,-6.58673</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="2">
         <v>10</v>
@@ -1159,14 +1424,18 @@
       <c r="E35">
         <v>-6.6002799999999997</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>34,2 Beaufield Drive Maynooth ,10,53.37414,-6.60028</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2">
         <v>18</v>
@@ -1177,14 +1446,18 @@
       <c r="E36">
         <v>-6.5361500000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>35,28 The Avenue Castletown Celbridge ,18,53.34514,-6.53615</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="2">
         <v>14</v>
@@ -1195,14 +1468,18 @@
       <c r="E37">
         <v>-6.67685</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>36,4 Abbey Park Grove Clane ,14,53.29206,-6.67685</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="2">
         <v>15</v>
@@ -1213,14 +1490,18 @@
       <c r="E38">
         <v>-6.54603</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>37,78 Crodaun Forest Park Celbridge ,15,53.35401,-6.54603</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2">
         <v>29</v>
@@ -1231,14 +1512,18 @@
       <c r="E39">
         <v>-6.5922599999999996</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>38,1 Kyldar House Manor Mills Maynooth ,29,53.38122,-6.59226</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="2">
         <v>22</v>
@@ -1249,13 +1534,17 @@
       <c r="E40">
         <v>-6.4831399999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>39,1002 Avondale Leixlip ,22,53.36869,-6.48314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="2">
         <v>5</v>
@@ -1266,8 +1555,216 @@
       <c r="E41">
         <v>-6.6004399999999999</v>
       </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>40,18 College Green Maynooth ,5,53.37247,-6.60044</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>